<commit_message>
Changed to start-end trimming
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingb\PycharmProjects\videosplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6203F434-5DC2-4371-9868-7EE35BF90FBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4C9A32-83F2-4475-BC42-A421E9E57375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>in/test.mp4</t>
   </si>
@@ -36,20 +36,32 @@
     <t>Output</t>
   </si>
   <si>
-    <t>N splits</t>
-  </si>
-  <si>
-    <t>out/test2/part{}.mp4</t>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>out/test2/part1.mp4</t>
+  </si>
+  <si>
+    <t>out/test2/part2.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,7 +381,7 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -379,19 +391,40 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>